<commit_message>
update: refactor extration path and pilot data concat
</commit_message>
<xml_diff>
--- a/src/main/static/rcbms/scripts/2021-pilot-cbms/references/sections/section_l.xlsx
+++ b/src/main/static/rcbms/scripts/2021-pilot-cbms/references/sections/section_l.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhasabdulsamad/Desktop/R Codes/2021-pilot-cbms/references/sections/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rcbms\scripts\2021-pilot-cbms\references\sections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072E24F7-5534-9E47-90D8-76DD2D406F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1820E4B8-7CD5-475D-80CC-0F08D8E007FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="section_l" sheetId="1" r:id="rId1"/>
@@ -290,9 +290,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>c_l01_not_in_vs_and_missing</t>
   </si>
   <si>
@@ -540,6 +537,9 @@
   </si>
   <si>
     <t>L18 all No</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1382,20 +1382,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
     <col min="4" max="4" width="71.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1412,12 +1412,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="str">
         <f>A2</f>
@@ -1427,12 +1427,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C66" si="0">A3</f>
@@ -1442,27 +1442,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>L02 not applicable</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1472,12 +1472,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1487,28 +1487,28 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>L05 missing or invalid</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
         <v>91</v>
       </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>L05 missing or invalid</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B8" t="s">
-        <v>92</v>
-      </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>L05 all No</v>
@@ -1517,222 +1517,222 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>L06 missing or invalid</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>L06-A not consistent</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>L06-B not consistent</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>L06-C not consistent</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>L06-D not consistent</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>L06-E not consistent</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>L06-F not consistent</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>L06-Z not consistent</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>L07-A missing or invalid</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>L07-B missing or invalid</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>L07-C missing or invalid</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>L07-D missing or invalid</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>L07-E missing or invalid</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>L07-F missing or invalid</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -1742,12 +1742,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -1757,12 +1757,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1772,12 +1772,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1787,28 +1787,28 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>L11 missing or invalid</v>
+      </c>
+      <c r="E27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" t="s">
         <v>111</v>
       </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>L11 missing or invalid</v>
-      </c>
-      <c r="E27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>167</v>
-      </c>
-      <c r="B28" t="s">
-        <v>112</v>
-      </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>L11 all No</v>
@@ -1817,12 +1817,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1832,12 +1832,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1850,12 +1850,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1865,12 +1865,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1880,12 +1880,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1895,12 +1895,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1910,27 +1910,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v>L16-L17 not applicable</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -1940,28 +1940,28 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
       <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>L18 missing or invalid</v>
+      </c>
+      <c r="E37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" t="s">
         <v>121</v>
       </c>
-      <c r="C37" t="str">
-        <f t="shared" si="0"/>
-        <v>L18 missing or invalid</v>
-      </c>
-      <c r="E37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" t="s">
-        <v>122</v>
-      </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v>L18 all No</v>
@@ -1970,12 +1970,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -1985,12 +1985,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -2003,12 +2003,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -2018,12 +2018,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -2033,12 +2033,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -2048,12 +2048,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -2063,27 +2063,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
         <v>L23-L24 not applicable</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -2093,12 +2093,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -2108,12 +2108,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -2123,12 +2123,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -2138,12 +2138,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
@@ -2153,12 +2153,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -2168,12 +2168,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -2183,12 +2183,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -2198,12 +2198,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -2213,12 +2213,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -2228,12 +2228,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -2243,12 +2243,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -2258,12 +2258,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -2273,12 +2273,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -2288,12 +2288,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -2303,12 +2303,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -2318,12 +2318,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -2333,12 +2333,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -2348,12 +2348,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -2363,12 +2363,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -2381,12 +2381,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -2396,12 +2396,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C81" si="1">A67</f>
@@ -2411,12 +2411,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -2426,12 +2426,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -2441,27 +2441,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>39</v>
       </c>
       <c r="B70" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v>L48-L49 not applicable</v>
       </c>
       <c r="E70" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -2471,12 +2471,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -2486,12 +2486,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -2501,12 +2501,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -2516,12 +2516,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -2531,12 +2531,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -2549,12 +2549,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -2564,64 +2564,64 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
         <v>L58 missing or invalid</v>
       </c>
       <c r="E78" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
         <v>L59 missing or invalid</v>
       </c>
       <c r="E79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
         <v>L60 missing or invalid</v>
       </c>
       <c r="E80" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>38</v>
       </c>
       <c r="B81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
         <v>L59-L60 not applicable</v>
       </c>
       <c r="E81" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>